<commit_message>
added auto-rerun until games==0
</commit_message>
<xml_diff>
--- a/data/TT/BlackOutDate-2020.xlsx
+++ b/data/TT/BlackOutDate-2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joel\Documents\GitHub\DjangoLeagueScheduler\data\TT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F6C5B6-456D-45A6-8A0B-8D0CC91ED187}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C81A377F-D84F-432D-9DFE-AA99D9981E82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="19632" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tablib Dataset" sheetId="1" r:id="rId1"/>
@@ -393,19 +393,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B93"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="24.20703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.21875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -413,292 +413,740 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
+        <v>301</v>
+      </c>
+      <c r="B2" s="2">
+        <v>43891</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
         <v>302</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B3" s="2">
         <v>43892</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>303</v>
+      </c>
+      <c r="B4" s="2">
+        <v>43893</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>304</v>
+      </c>
+      <c r="B5" s="2">
+        <v>43894</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>305</v>
+      </c>
+      <c r="B6" s="2">
+        <v>43895</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>306</v>
+      </c>
+      <c r="B7" s="2">
+        <v>43896</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>307</v>
+      </c>
+      <c r="B8" s="2">
+        <v>43897</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>308</v>
+      </c>
+      <c r="B9" s="2">
+        <v>43898</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>309</v>
+      </c>
+      <c r="B10" s="2">
+        <v>43899</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>310</v>
+      </c>
+      <c r="B11" s="2">
+        <v>43900</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>311</v>
+      </c>
+      <c r="B12" s="2">
+        <v>43901</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>312</v>
+      </c>
+      <c r="B13" s="2">
+        <v>43902</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>313</v>
+      </c>
+      <c r="B14" s="2">
+        <v>43903</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>314</v>
+      </c>
+      <c r="B15" s="2">
+        <v>43904</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16">
         <v>315</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B16" s="2">
         <v>43905</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17">
         <v>316</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B17" s="2">
         <v>43906</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18">
         <v>317</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B18" s="2">
         <v>43907</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19">
         <v>318</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B19" s="2">
         <v>43908</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20">
         <v>319</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B20" s="2">
         <v>43909</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>320</v>
+      </c>
+      <c r="B21" s="2">
+        <v>43910</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>321</v>
+      </c>
+      <c r="B22" s="2">
+        <v>43911</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>322</v>
+      </c>
+      <c r="B23" s="2">
+        <v>43912</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24">
         <v>323</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B24" s="2">
         <v>43913</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25">
         <v>324</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B25" s="2">
         <v>43914</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>325</v>
+      </c>
+      <c r="B26" s="2">
+        <v>43915</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27">
         <v>326</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B27" s="2">
         <v>43916</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>327</v>
+      </c>
+      <c r="B28" s="2">
+        <v>43917</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29">
         <v>328</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B29" s="2">
         <v>43918</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>329</v>
+      </c>
+      <c r="B30" s="2">
+        <v>43919</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31">
         <v>330</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B31" s="2">
         <v>43920</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32">
         <v>331</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B32" s="2">
         <v>43921</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>401</v>
+      </c>
+      <c r="B33" s="2">
+        <v>43922</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>402</v>
+      </c>
+      <c r="B34" s="2">
+        <v>43923</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35">
         <v>403</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B35" s="2">
         <v>43924</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>404</v>
+      </c>
+      <c r="B36" s="2">
+        <v>43925</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>405</v>
+      </c>
+      <c r="B37" s="2">
+        <v>43926</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38">
         <v>406</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B38" s="2">
         <v>43927</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39">
         <v>407</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B39" s="2">
         <v>43928</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40">
         <v>408</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B40" s="2">
         <v>43929</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41">
         <v>409</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B41" s="2">
         <v>43930</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>410</v>
+      </c>
+      <c r="B42" s="2">
+        <v>43931</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>411</v>
+      </c>
+      <c r="B43" s="2">
+        <v>43932</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>412</v>
+      </c>
+      <c r="B44" s="2">
+        <v>43933</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45">
         <v>413</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B45" s="2">
         <v>43934</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46">
         <v>414</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B46" s="2">
         <v>43935</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>415</v>
+      </c>
+      <c r="B47" s="2">
+        <v>43936</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>416</v>
+      </c>
+      <c r="B48" s="2">
+        <v>43937</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>417</v>
+      </c>
+      <c r="B49" s="2">
+        <v>43938</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50">
         <v>418</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B50" s="2">
         <v>43939</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51">
         <v>419</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B51" s="2">
         <v>43940</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52">
         <v>420</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B52" s="2">
         <v>43941</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53">
         <v>421</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B53" s="2">
         <v>43942</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>422</v>
+      </c>
+      <c r="B54" s="2">
+        <v>43943</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>423</v>
+      </c>
+      <c r="B55" s="2">
+        <v>43944</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>424</v>
+      </c>
+      <c r="B56" s="2">
+        <v>43945</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>425</v>
+      </c>
+      <c r="B57" s="2">
+        <v>43946</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>426</v>
+      </c>
+      <c r="B58" s="2">
+        <v>43947</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59">
         <v>427</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B59" s="2">
         <v>43948</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60">
         <v>428</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B60" s="2">
         <v>43949</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61">
         <v>429</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B61" s="2">
         <v>43950</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>430</v>
+      </c>
+      <c r="B62" s="2">
+        <v>43951</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>501</v>
+      </c>
+      <c r="B63" s="2">
+        <v>43952</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64">
         <v>502</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B64" s="2">
         <v>43953</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>503</v>
+      </c>
+      <c r="B65" s="2">
+        <v>43954</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66">
         <v>504</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B66" s="2">
         <v>43955</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67">
         <v>505</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B67" s="2">
         <v>43956</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68">
         <v>506</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B68" s="2">
         <v>43957</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>507</v>
+      </c>
+      <c r="B69" s="2">
+        <v>43958</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70">
         <v>508</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B70" s="2">
         <v>43959</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71">
         <v>509</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B71" s="2">
         <v>43960</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>510</v>
+      </c>
+      <c r="B72" s="2">
+        <v>43961</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73">
         <v>511</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B73" s="2">
         <v>43962</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74">
         <v>512</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B74" s="2">
         <v>43963</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>513</v>
+      </c>
+      <c r="B75" s="2">
+        <v>43964</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>514</v>
+      </c>
+      <c r="B76" s="2">
+        <v>43965</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>515</v>
+      </c>
+      <c r="B77" s="2">
+        <v>43966</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>516</v>
+      </c>
+      <c r="B78" s="2">
+        <v>43967</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>517</v>
+      </c>
+      <c r="B79" s="2">
+        <v>43968</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80">
         <v>518</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B80" s="2">
         <v>43969</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81">
         <v>519</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B81" s="2">
         <v>43970</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>520</v>
+      </c>
+      <c r="B82" s="2">
+        <v>43971</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>521</v>
+      </c>
+      <c r="B83" s="2">
+        <v>43972</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>522</v>
+      </c>
+      <c r="B84" s="2">
+        <v>43973</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>523</v>
+      </c>
+      <c r="B85" s="2">
+        <v>43974</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>524</v>
+      </c>
+      <c r="B86" s="2">
+        <v>43975</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>525</v>
+      </c>
+      <c r="B87" s="2">
+        <v>43976</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>526</v>
+      </c>
+      <c r="B88" s="2">
+        <v>43977</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>527</v>
+      </c>
+      <c r="B89" s="2">
+        <v>43978</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>528</v>
+      </c>
+      <c r="B90" s="2">
+        <v>43979</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>529</v>
+      </c>
+      <c r="B91" s="2">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>530</v>
+      </c>
+      <c r="B92" s="2">
+        <v>43981</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>531</v>
+      </c>
+      <c r="B93" s="2">
+        <v>43982</v>
       </c>
     </row>
   </sheetData>

</xml_diff>